<commit_message>
Update 2021 data and everything with it
</commit_message>
<xml_diff>
--- a/data/tower_count/tower_count_2021.xlsx
+++ b/data/tower_count/tower_count_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejgna\Documents\project-eleanor-and-wriley\data\tower_count\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA85F09-3472-430F-9193-5B014BBE7835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CD7D19-8957-4455-883B-BE38020BEBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>date</t>
   </si>
@@ -46,6 +46,75 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>3 DCCO, 2 RAZO</t>
+  </si>
+  <si>
+    <t>10 DCCO, 1 RAZO</t>
+  </si>
+  <si>
+    <t>1 BAEA, 6 corvid</t>
+  </si>
+  <si>
+    <t>1 ATPU</t>
+  </si>
+  <si>
+    <t>4 DCCO, 1 ATPU</t>
+  </si>
+  <si>
+    <t>3 corvid, 1 RAZO</t>
+  </si>
+  <si>
+    <t>3 RAZO</t>
+  </si>
+  <si>
+    <t>1 NOGA</t>
+  </si>
+  <si>
+    <t>1 COTE</t>
+  </si>
+  <si>
+    <t>1 BAEA, 5 corvid</t>
+  </si>
+  <si>
+    <t>1 RAZO</t>
+  </si>
+  <si>
+    <t>2 ATPU</t>
+  </si>
+  <si>
+    <t>1 ATPU, 1 RAZO, 4 corvid</t>
+  </si>
+  <si>
+    <t>2 ATPU, 6 DCCO, 1 RAZO</t>
+  </si>
+  <si>
+    <t>3 RAZO, 2 ATPU</t>
+  </si>
+  <si>
+    <t>3 ATPU, 2 RAZO</t>
+  </si>
+  <si>
+    <t>3 NOGA</t>
+  </si>
+  <si>
+    <t>6 ATPU, 2 DCCO</t>
+  </si>
+  <si>
+    <t>4 ATPU</t>
+  </si>
+  <si>
+    <t>57 WISP, 1 ATPU, 5 porpoise, 3 RAZO</t>
+  </si>
+  <si>
+    <t>15 ATPU, 1 COMU, 7 RAZO</t>
+  </si>
+  <si>
+    <t>26 ATPU, 6 NOGA</t>
+  </si>
+  <si>
+    <t>30 WISP</t>
   </si>
 </sst>
 </file>
@@ -364,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,6 +486,9 @@
       <c r="F2">
         <v>123</v>
       </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -437,6 +509,9 @@
       <c r="F3">
         <v>155</v>
       </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -457,6 +532,9 @@
       <c r="F4">
         <v>102</v>
       </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -477,6 +555,9 @@
       <c r="F5">
         <v>161</v>
       </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -497,6 +578,9 @@
       <c r="F6">
         <v>134</v>
       </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -517,6 +601,9 @@
       <c r="F7">
         <v>90</v>
       </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -537,6 +624,9 @@
       <c r="F8">
         <v>113</v>
       </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -557,6 +647,9 @@
       <c r="F9">
         <v>153</v>
       </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -577,6 +670,9 @@
       <c r="F10">
         <v>181</v>
       </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -597,6 +693,9 @@
       <c r="F11">
         <v>91</v>
       </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -617,6 +716,9 @@
       <c r="F12">
         <v>145</v>
       </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -657,6 +759,9 @@
       <c r="F14">
         <v>112</v>
       </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -677,6 +782,9 @@
       <c r="F15">
         <v>123</v>
       </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -697,8 +805,11 @@
       <c r="F16">
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44375</v>
       </c>
@@ -717,8 +828,11 @@
       <c r="F17">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44376</v>
       </c>
@@ -737,8 +851,11 @@
       <c r="F18">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44377</v>
       </c>
@@ -757,8 +874,11 @@
       <c r="F19">
         <v>95</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44378</v>
       </c>
@@ -778,7 +898,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44380</v>
       </c>
@@ -797,8 +917,11 @@
       <c r="F21">
         <v>156</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44381</v>
       </c>
@@ -818,7 +941,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44382</v>
       </c>
@@ -837,8 +960,11 @@
       <c r="F23">
         <v>153</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44384</v>
       </c>
@@ -857,8 +983,11 @@
       <c r="F24">
         <v>158</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44385</v>
       </c>
@@ -878,7 +1007,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44387</v>
       </c>
@@ -898,7 +1027,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44388</v>
       </c>
@@ -917,8 +1046,11 @@
       <c r="F27">
         <v>234</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44389</v>
       </c>
@@ -937,8 +1069,11 @@
       <c r="F28">
         <v>198</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44390</v>
       </c>
@@ -958,7 +1093,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44391</v>
       </c>
@@ -978,7 +1113,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44393</v>
       </c>
@@ -998,7 +1133,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44394</v>
       </c>
@@ -1018,17 +1153,111 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>44395</v>
+      </c>
+      <c r="B33">
+        <v>584</v>
+      </c>
+      <c r="C33">
+        <v>41</v>
+      </c>
+      <c r="D33">
+        <v>35</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>44399</v>
+      </c>
+      <c r="B34">
+        <v>599</v>
+      </c>
+      <c r="C34">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>72</v>
+      </c>
+      <c r="E34">
+        <v>9</v>
+      </c>
+      <c r="F34">
+        <v>146</v>
+      </c>
+      <c r="G34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>44400</v>
+      </c>
+      <c r="B35">
+        <v>565</v>
+      </c>
+      <c r="C35">
+        <v>53</v>
+      </c>
+      <c r="D35">
+        <v>83</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>151</v>
+      </c>
+      <c r="G35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>44401</v>
+      </c>
+      <c r="B36">
+        <v>596</v>
+      </c>
+      <c r="C36">
+        <v>42</v>
+      </c>
+      <c r="D36">
+        <v>96</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>44402</v>
+      </c>
+      <c r="B37">
+        <v>518</v>
+      </c>
+      <c r="C37">
+        <v>52</v>
+      </c>
+      <c r="D37">
+        <v>54</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>